<commit_message>
imported more ipynb and nyc-taxi
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Developer/e2e_mlops_aws/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CE21A6-D1CE-D14F-B3EC-70D5A43A728D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD874903-F6E7-ED48-BB55-2C4FE3354B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6500" yWindow="4280" windowWidth="28100" windowHeight="17440" xr2:uid="{DEA1F039-2A23-7C42-A89A-87C064EC9890}"/>
+    <workbookView xWindow="6500" yWindow="4280" windowWidth="28100" windowHeight="17440" activeTab="1" xr2:uid="{DEA1F039-2A23-7C42-A89A-87C064EC9890}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
   <si>
     <t xml:space="preserve">Identifying groups of customers with the same buying patterns </t>
   </si>
@@ -123,28 +124,90 @@
   </si>
   <si>
     <t>Imputation</t>
+  </si>
+  <si>
+    <t>Creating a Regression Model with Azure ML Designer</t>
+  </si>
+  <si>
+    <t>A Cloud Guru</t>
+  </si>
+  <si>
+    <t>Creating a Classification Model with Azure ML Designer</t>
+  </si>
+  <si>
+    <t>Classifying Images with Azure Custom Vision</t>
+  </si>
+  <si>
+    <t>Analyzing Faces with Azure AI</t>
+  </si>
+  <si>
+    <t>Creating a Clustering Model with Azure ML Designer</t>
+  </si>
+  <si>
+    <t>Object Detection with Azure Custom Vision</t>
+  </si>
+  <si>
+    <t>Analyzing Text with Text Analytics on Azure</t>
+  </si>
+  <si>
+    <t>Create a Basic Pipeline in Azure Machine Learning Studio</t>
+  </si>
+  <si>
+    <t>Identifying Iris Plants Using Machine Learning</t>
+  </si>
+  <si>
+    <t>GCP</t>
+  </si>
+  <si>
+    <t>Azure</t>
+  </si>
+  <si>
+    <t>Using Python ML for Predictive Analytics</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>Automatically Processing Data in S3 Using Lambda</t>
+  </si>
+  <si>
+    <t>Run a Batch Inferencing Pipeline and Obtain Outputs</t>
+  </si>
+  <si>
+    <t>Classify Images Using TensorFlow</t>
+  </si>
+  <si>
+    <t>Loading Data from TensorFlow Datasets</t>
+  </si>
+  <si>
+    <t>Performing OCR on an Image Using the .NET SDK</t>
+  </si>
+  <si>
+    <t>Visualizing Anomalies in Kibana 7.6</t>
+  </si>
+  <si>
+    <t>AWS-Kibana</t>
+  </si>
+  <si>
+    <t>Predicting Sequences Using TensorFlow</t>
+  </si>
+  <si>
+    <t>Generating Text Using TensorFlow</t>
+  </si>
+  <si>
+    <t>Detecting Faces within Images Using the .NET SDK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Cascadia Code"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF3D3B49"/>
-      <name val="Noto Serif"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF3D3B49"/>
-      <name val="Noto Serif"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,10 +230,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,221 +566,439 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E2171E-D264-7D40-A31C-3EB3F82D1FDE}">
-  <dimension ref="A4:E47"/>
+  <dimension ref="A4:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="132.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="2:5" ht="24" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="24" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="D11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
+      <c r="D12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="E13" t="s">
+      <c r="D13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="E14" t="s">
+      <c r="D14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="D18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="E19" t="s">
+      <c r="D19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="E20" t="s">
+      <c r="D20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="D24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>16</v>
       </c>
-      <c r="E25" t="s">
+      <c r="D25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>16</v>
       </c>
-      <c r="E26" t="s">
+      <c r="D26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>16</v>
       </c>
-      <c r="E27" t="s">
+      <c r="D27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>13</v>
       </c>
       <c r="B32" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="D32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>13</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
       </c>
-      <c r="E33" t="s">
+      <c r="D33" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>13</v>
       </c>
       <c r="B34" t="s">
         <v>14</v>
       </c>
-      <c r="E34" t="s">
+      <c r="D34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>13</v>
       </c>
       <c r="B36" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="D36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>13</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
       </c>
-      <c r="E37" t="s">
+      <c r="D37" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>13</v>
       </c>
       <c r="B38" t="s">
         <v>15</v>
       </c>
-      <c r="E38" t="s">
+      <c r="D38" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="19" x14ac:dyDescent="0.3">
-      <c r="E45" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E46" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E47" t="s">
-        <v>5</v>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545C6B1B-2F98-2843-AF22-A4259C8ABF32}">
+  <dimension ref="B2:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>